<commit_message>
Actualizacion en dias de nomina y gral
Varios archivos para los dias de nomina e impresiones en prima de
vacaciones
</commit_message>
<xml_diff>
--- a/Liquidacion_20143370.xlsx
+++ b/Liquidacion_20143370.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>UNIVERSIDAD DE LAGUAJIRA</t>
   </si>
@@ -42,19 +42,25 @@
     <t>MESES</t>
   </si>
   <si>
-    <t>Sueldo</t>
-  </si>
-  <si>
-    <t>Subsidio Transporte</t>
-  </si>
-  <si>
-    <t>Subsidio Alimentacion</t>
-  </si>
-  <si>
-    <t>Bon. de Servicios</t>
-  </si>
-  <si>
-    <t>Prima de Servicios</t>
+    <t>DEVENGADO</t>
+  </si>
+  <si>
+    <t>NETO</t>
+  </si>
+  <si>
+    <t>SUELDO</t>
+  </si>
+  <si>
+    <t>AUX. TRASNPORTE</t>
+  </si>
+  <si>
+    <t>AUX. ALIMENTACION</t>
+  </si>
+  <si>
+    <t>1/12 BON. DE SERVICIOS</t>
+  </si>
+  <si>
+    <t>1/12 P. DE SERVICIOS</t>
   </si>
   <si>
     <t>TOTAL VACACIONES</t>
@@ -69,7 +75,7 @@
     <t>PRIMA NAVIDAD</t>
   </si>
   <si>
-    <t>Prima de Vacaciones</t>
+    <t>1/12 P. DE VACACIONES</t>
   </si>
   <si>
     <t>TOTAL PRIMA NAVIDAD</t>
@@ -136,7 +142,7 @@
       </gradientFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border/>
     <border>
       <left style="thick">
@@ -149,6 +155,20 @@
         <color rgb="000000"/>
       </top>
       <bottom style="thick">
+        <color rgb="000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="dashed">
+        <color rgb="000000"/>
+      </left>
+      <right style="dashed">
+        <color rgb="000000"/>
+      </right>
+      <top style="dashed">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="dashed">
         <color rgb="000000"/>
       </bottom>
     </border>
@@ -161,6 +181,20 @@
       <left style="thick">
         <color rgb="000000"/>
       </left>
+      <right style="dashed">
+        <color rgb="000000"/>
+      </right>
+      <top style="dashed">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="dashed">
+        <color rgb="000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="000000"/>
+      </left>
       <bottom style="thick">
         <color rgb="000000"/>
       </bottom>
@@ -176,10 +210,16 @@
       </right>
     </border>
     <border>
+      <left style="dashed">
+        <color rgb="000000"/>
+      </left>
       <right style="thick">
         <color rgb="000000"/>
       </right>
-      <bottom style="thick">
+      <top style="dashed">
+        <color rgb="000000"/>
+      </top>
+      <bottom style="dashed">
         <color rgb="000000"/>
       </bottom>
     </border>
@@ -187,32 +227,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="2" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="2" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="1" numFmtId="3" fillId="2" borderId="1" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="3" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="4" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="5" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="6" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="7" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="8" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="6" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="3" fillId="0" borderId="4" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -523,6 +575,7 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="true" style="0"/>
+    <col min="5" max="5" width="13" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
@@ -558,433 +611,486 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="B6" s="3"/>
+      <c r="B6" s="6"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7"/>
-      <c r="E7" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" s="6"/>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2582170.9090909</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" s="4">
         <v>1420194</v>
-      </c>
-      <c r="D8"/>
-      <c r="E8">
-        <v>9</v>
       </c>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="4">
+        <v>106467.27272727</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" s="4">
         <v>58557</v>
       </c>
-      <c r="D9"/>
-      <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
-      <c r="H9" s="6"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4">
+        <v>47550.909090909</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" s="4">
         <v>26153</v>
       </c>
-      <c r="D10"/>
-      <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
       <c r="D11"/>
-      <c r="E11"/>
+      <c r="E11" s="4"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="B12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4">
+        <v>63307.272727273</v>
+      </c>
+      <c r="D12"/>
+      <c r="E12" s="4">
         <v>34819</v>
       </c>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="4">
+        <v>233445.45454545</v>
+      </c>
+      <c r="D13"/>
+      <c r="E13" s="4">
         <v>128395</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
       <c r="D14"/>
-      <c r="E14"/>
+      <c r="E14" s="4"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="B15" s="4"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="7">
+      <c r="B15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="5">
         <v>1668118</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16"/>
-      <c r="E16" t="s">
+      <c r="B16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16" s="6"/>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:8">
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2582170.6666667</v>
+      </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4">
         <v>968314</v>
-      </c>
-      <c r="D17"/>
-      <c r="E17">
-        <v>9</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4">
+        <v>106466.66666667</v>
+      </c>
+      <c r="D18"/>
+      <c r="E18" s="4">
         <v>39925</v>
       </c>
-      <c r="D18"/>
-      <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="B19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4">
+        <v>47552</v>
+      </c>
+      <c r="D19"/>
+      <c r="E19" s="4">
         <v>17832</v>
       </c>
-      <c r="D19"/>
-      <c r="E19"/>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
       <c r="D20"/>
-      <c r="E20"/>
+      <c r="E20" s="4"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="B21" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="4">
+        <v>63306.666666667</v>
+      </c>
+      <c r="D21"/>
+      <c r="E21" s="4">
         <v>23740</v>
       </c>
-      <c r="D21"/>
-      <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="B22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="2">
+      <c r="B22" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4">
+        <v>233445.33333333</v>
+      </c>
+      <c r="D22"/>
+      <c r="E22" s="4">
         <v>87542</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
       <c r="D23"/>
-      <c r="E23"/>
+      <c r="E23" s="4"/>
       <c r="F23"/>
       <c r="G23"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="7">
+      <c r="B24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="5">
         <v>1137353</v>
       </c>
     </row>
     <row r="25" spans="1:8">
-      <c r="B25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="2"/>
-      <c r="D25"/>
-      <c r="E25" t="s">
+      <c r="B25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F25"/>
-      <c r="G25"/>
-      <c r="H25" s="6"/>
+      <c r="E25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="11" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
-      <c r="B26" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1936628</v>
-      </c>
-      <c r="D26"/>
-      <c r="E26">
-        <v>9</v>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2582169.6</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2151808</v>
       </c>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26" s="6"/>
+      <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="B27" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="2">
-        <v>79850</v>
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4">
+        <v>106467.6</v>
       </c>
       <c r="D27"/>
-      <c r="E27"/>
+      <c r="E27" s="4">
+        <v>88723</v>
+      </c>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" s="6"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="B28" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C28" s="2">
-        <v>35663</v>
+      <c r="B28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="4">
+        <v>47551.2</v>
       </c>
       <c r="D28"/>
-      <c r="E28"/>
+      <c r="E28" s="4">
+        <v>39626</v>
+      </c>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28" s="6"/>
+      <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="B29" s="3"/>
-      <c r="C29" s="2"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="4"/>
       <c r="D29"/>
-      <c r="E29"/>
+      <c r="E29" s="4"/>
       <c r="F29"/>
       <c r="G29"/>
-      <c r="H29" s="6"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="B30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="2">
-        <v>47480</v>
+      <c r="B30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4">
+        <v>63307.2</v>
       </c>
       <c r="D30"/>
-      <c r="E30"/>
+      <c r="E30" s="4">
+        <v>52756</v>
+      </c>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="H30" s="6"/>
+      <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="B31" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2">
-        <v>175085</v>
+      <c r="B31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="4">
+        <v>233445.6</v>
       </c>
       <c r="D31"/>
-      <c r="E31"/>
+      <c r="E31" s="4">
+        <v>194538</v>
+      </c>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="H31" s="6"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="B32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="2">
-        <v>93550</v>
+      <c r="B32" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="4">
+        <v>124734</v>
       </c>
       <c r="D32"/>
-      <c r="E32"/>
+      <c r="E32" s="4">
+        <v>103945</v>
+      </c>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" s="6"/>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="B33" s="3"/>
+      <c r="B33" s="6"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33" s="6"/>
+      <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="B34" s="4"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="7">
-        <v>2368256</v>
+      <c r="B34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="5">
+        <v>2631396</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="F36" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G36"/>
-      <c r="H36" s="2">
-        <v>5173727</v>
+      <c r="H36" s="4">
+        <v>5436867</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="F38" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G38"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="40" spans="1:8">
       <c r="F40" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G40"/>
-      <c r="H40" s="2">
-        <v>5173727</v>
+      <c r="H40" s="4">
+        <v>5436867</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="B43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E43"/>
       <c r="G43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H43"/>
     </row>
     <row r="45" spans="1:8">
       <c r="B45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E45"/>
       <c r="G45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H45"/>
     </row>
     <row r="47" spans="1:8">
       <c r="B47" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E47"/>
       <c r="G47" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H47"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="B34:C34"/>
     <mergeCell ref="F36:G36"/>
     <mergeCell ref="F38:G38"/>
     <mergeCell ref="F40:G40"/>

</xml_diff>